<commit_message>
Upload IO project in github
</commit_message>
<xml_diff>
--- a/App11.xlsx
+++ b/App11.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\farid\ordmission11022019\Gestion_Ord_Mission\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6990"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="152511" iterate="1" iterateCount="2" iterateDelta="0.01"/>
+  <calcPr calcId="124519" iterate="1" iterateCount="2" iterateDelta="0.01"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -517,11 +512,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-dd\-mm"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1147,15 +1142,186 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1165,176 +1331,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1408,41 +1433,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1761,7 +1756,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Feuil1"/>
@@ -2033,21 +2028,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36:U36"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="64" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11.42578125" style="64"/>
@@ -2074,7 +2069,7 @@
     <col min="23" max="16384" width="11.42578125" style="64"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="B1" s="85"/>
       <c r="C1" s="91"/>
       <c r="D1" s="91"/>
@@ -2085,7 +2080,7 @@
       <c r="I1" s="91"/>
       <c r="J1" s="91"/>
     </row>
-    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="B2" s="91"/>
       <c r="C2" s="91"/>
       <c r="D2" s="91"/>
@@ -2101,7 +2096,7 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15.75" customHeight="1">
       <c r="B3" s="91"/>
       <c r="C3" s="91"/>
       <c r="D3" s="91"/>
@@ -2112,49 +2107,49 @@
       <c r="I3" s="91"/>
       <c r="J3" s="91"/>
       <c r="K3" s="92"/>
-      <c r="P3" s="176" t="s">
+      <c r="P3" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="176"/>
-      <c r="R3" s="176"/>
-      <c r="S3" s="176"/>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+    </row>
+    <row r="4" spans="1:22" ht="15.75">
       <c r="B4" s="91"/>
-      <c r="C4" s="177" t="s">
+      <c r="C4" s="127" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
-      <c r="H4" s="134"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
       <c r="I4" s="91"/>
       <c r="J4" s="91"/>
       <c r="K4" s="92"/>
-      <c r="P4" s="176"/>
-      <c r="Q4" s="176"/>
-      <c r="R4" s="176"/>
-      <c r="S4" s="176"/>
-    </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="126"/>
+      <c r="Q4" s="126"/>
+      <c r="R4" s="126"/>
+      <c r="S4" s="126"/>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" customHeight="1">
       <c r="B5" s="91"/>
-      <c r="C5" s="134"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="134"/>
-      <c r="F5" s="134"/>
-      <c r="G5" s="134"/>
-      <c r="H5" s="134"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
       <c r="I5" s="91"/>
       <c r="J5" s="91"/>
       <c r="K5" s="92"/>
-      <c r="T5" s="135" t="s">
+      <c r="T5" s="129" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="135"/>
-      <c r="V5" s="135"/>
-    </row>
-    <row r="6" spans="1:22" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U5" s="129"/>
+      <c r="V5" s="129"/>
+    </row>
+    <row r="6" spans="1:22" ht="16.5" customHeight="1" thickBot="1">
       <c r="B6" s="91"/>
       <c r="C6" s="85"/>
       <c r="D6" s="85"/>
@@ -2172,11 +2167,11 @@
       <c r="Q6" s="62"/>
       <c r="R6" s="62"/>
       <c r="S6" s="62"/>
-      <c r="T6" s="178"/>
-      <c r="U6" s="178"/>
-      <c r="V6" s="178"/>
-    </row>
-    <row r="7" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T6" s="130"/>
+      <c r="U6" s="130"/>
+      <c r="V6" s="130"/>
+    </row>
+    <row r="7" spans="1:22" ht="16.5" thickBot="1">
       <c r="B7" s="91"/>
       <c r="C7" s="85"/>
       <c r="D7" s="85"/>
@@ -2190,26 +2185,26 @@
       <c r="L7" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="163"/>
+      <c r="M7" s="131"/>
       <c r="N7" s="59" t="s">
         <v>36</v>
       </c>
       <c r="O7" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="180" t="s">
+      <c r="P7" s="133" t="s">
         <v>38</v>
       </c>
-      <c r="Q7" s="180"/>
-      <c r="R7" s="180"/>
-      <c r="S7" s="181"/>
-      <c r="T7" s="154" t="s">
+      <c r="Q7" s="133"/>
+      <c r="R7" s="133"/>
+      <c r="S7" s="134"/>
+      <c r="T7" s="135" t="s">
         <v>39</v>
       </c>
-      <c r="U7" s="155"/>
-      <c r="V7" s="156"/>
-    </row>
-    <row r="8" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U7" s="136"/>
+      <c r="V7" s="137"/>
+    </row>
+    <row r="8" spans="1:22" ht="16.5" thickBot="1">
       <c r="B8" s="91"/>
       <c r="C8" s="91"/>
       <c r="D8" s="91"/>
@@ -2220,24 +2215,24 @@
       <c r="I8" s="91"/>
       <c r="J8" s="91"/>
       <c r="K8" s="92"/>
-      <c r="L8" s="161"/>
-      <c r="M8" s="179"/>
-      <c r="N8" s="148">
+      <c r="L8" s="138"/>
+      <c r="M8" s="132"/>
+      <c r="N8" s="140">
         <f>P8*O8</f>
         <v>0</v>
       </c>
-      <c r="O8" s="148"/>
-      <c r="P8" s="148"/>
-      <c r="Q8" s="148"/>
-      <c r="R8" s="148"/>
-      <c r="S8" s="182"/>
+      <c r="O8" s="140"/>
+      <c r="P8" s="140"/>
+      <c r="Q8" s="140"/>
+      <c r="R8" s="140"/>
+      <c r="S8" s="141"/>
       <c r="T8" s="93"/>
-      <c r="U8" s="183" t="s">
+      <c r="U8" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="V8" s="184"/>
-    </row>
-    <row r="9" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V8" s="143"/>
+    </row>
+    <row r="9" spans="1:22" ht="16.5" thickBot="1">
       <c r="B9" s="91"/>
       <c r="C9" s="91"/>
       <c r="D9" s="91"/>
@@ -2248,154 +2243,154 @@
       <c r="I9" s="91"/>
       <c r="J9" s="91"/>
       <c r="K9" s="92"/>
-      <c r="L9" s="162"/>
-      <c r="M9" s="179"/>
-      <c r="N9" s="148"/>
-      <c r="O9" s="148"/>
-      <c r="P9" s="148"/>
-      <c r="Q9" s="148"/>
-      <c r="R9" s="148"/>
-      <c r="S9" s="182"/>
-      <c r="T9" s="185"/>
-      <c r="U9" s="165"/>
+      <c r="L9" s="139"/>
+      <c r="M9" s="132"/>
+      <c r="N9" s="140"/>
+      <c r="O9" s="140"/>
+      <c r="P9" s="140"/>
+      <c r="Q9" s="140"/>
+      <c r="R9" s="140"/>
+      <c r="S9" s="141"/>
+      <c r="T9" s="144"/>
+      <c r="U9" s="145"/>
       <c r="V9" s="94" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="16.5" thickBot="1">
       <c r="B10" s="91"/>
       <c r="C10" s="91"/>
-      <c r="D10" s="186" t="s">
+      <c r="D10" s="146" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="187"/>
-      <c r="F10" s="187"/>
-      <c r="G10" s="145"/>
+      <c r="E10" s="147"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="148"/>
       <c r="H10" s="91"/>
       <c r="I10" s="91"/>
       <c r="J10" s="91"/>
       <c r="K10" s="92"/>
       <c r="L10" s="90"/>
-      <c r="M10" s="179"/>
+      <c r="M10" s="132"/>
       <c r="N10" s="89">
         <f>O10*P10</f>
         <v>0</v>
       </c>
       <c r="O10" s="96"/>
-      <c r="P10" s="182"/>
-      <c r="Q10" s="171"/>
-      <c r="R10" s="171"/>
-      <c r="S10" s="172"/>
-      <c r="T10" s="182"/>
-      <c r="U10" s="172"/>
+      <c r="P10" s="141"/>
+      <c r="Q10" s="152"/>
+      <c r="R10" s="152"/>
+      <c r="S10" s="153"/>
+      <c r="T10" s="141"/>
+      <c r="U10" s="153"/>
       <c r="V10" s="60" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="16.5" thickBot="1">
       <c r="B11" s="91"/>
       <c r="C11" s="91"/>
-      <c r="D11" s="146"/>
-      <c r="E11" s="188"/>
-      <c r="F11" s="188"/>
-      <c r="G11" s="147"/>
+      <c r="D11" s="149"/>
+      <c r="E11" s="150"/>
+      <c r="F11" s="150"/>
+      <c r="G11" s="151"/>
       <c r="H11" s="91"/>
       <c r="I11" s="91"/>
       <c r="J11" s="91"/>
       <c r="K11" s="92"/>
       <c r="L11" s="90"/>
-      <c r="M11" s="179"/>
+      <c r="M11" s="132"/>
       <c r="N11" s="89">
         <f>O11*P11</f>
         <v>0</v>
       </c>
       <c r="O11" s="96"/>
-      <c r="P11" s="182"/>
-      <c r="Q11" s="171"/>
-      <c r="R11" s="171"/>
-      <c r="S11" s="172"/>
-      <c r="T11" s="158" t="s">
+      <c r="P11" s="141"/>
+      <c r="Q11" s="152"/>
+      <c r="R11" s="152"/>
+      <c r="S11" s="153"/>
+      <c r="T11" s="154" t="s">
         <v>44</v>
       </c>
-      <c r="U11" s="159"/>
-      <c r="V11" s="160"/>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="140" t="s">
+      <c r="U11" s="155"/>
+      <c r="V11" s="156"/>
+    </row>
+    <row r="12" spans="1:22" ht="15.75">
+      <c r="A12" s="166" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="140"/>
-      <c r="C12" s="140"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="151" t="s">
+      <c r="B12" s="166"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="166"/>
+      <c r="E12" s="167" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="140"/>
-      <c r="G12" s="140"/>
-      <c r="H12" s="140"/>
-      <c r="I12" s="140"/>
-      <c r="J12" s="152" t="s">
+      <c r="F12" s="166"/>
+      <c r="G12" s="166"/>
+      <c r="H12" s="166"/>
+      <c r="I12" s="166"/>
+      <c r="J12" s="168" t="s">
         <v>95</v>
       </c>
       <c r="K12" s="92"/>
-      <c r="L12" s="161"/>
-      <c r="M12" s="179"/>
-      <c r="N12" s="161">
+      <c r="L12" s="138"/>
+      <c r="M12" s="132"/>
+      <c r="N12" s="138">
         <f>O12*Q12</f>
         <v>0</v>
       </c>
-      <c r="O12" s="161"/>
+      <c r="O12" s="138"/>
       <c r="P12" s="97"/>
-      <c r="Q12" s="163"/>
-      <c r="R12" s="163"/>
-      <c r="S12" s="164"/>
-      <c r="T12" s="167" t="s">
+      <c r="Q12" s="131"/>
+      <c r="R12" s="131"/>
+      <c r="S12" s="157"/>
+      <c r="T12" s="159" t="s">
         <v>46</v>
       </c>
-      <c r="U12" s="168"/>
-      <c r="V12" s="169"/>
-    </row>
-    <row r="13" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="140"/>
-      <c r="B13" s="140"/>
-      <c r="C13" s="140"/>
-      <c r="D13" s="140"/>
-      <c r="E13" s="151"/>
-      <c r="F13" s="140"/>
-      <c r="G13" s="140"/>
-      <c r="H13" s="140"/>
-      <c r="I13" s="140"/>
-      <c r="J13" s="152"/>
+      <c r="U12" s="160"/>
+      <c r="V12" s="161"/>
+    </row>
+    <row r="13" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A13" s="166"/>
+      <c r="B13" s="166"/>
+      <c r="C13" s="166"/>
+      <c r="D13" s="166"/>
+      <c r="E13" s="167"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="168"/>
       <c r="K13" s="92"/>
-      <c r="L13" s="162"/>
-      <c r="M13" s="179"/>
-      <c r="N13" s="162"/>
-      <c r="O13" s="162"/>
+      <c r="L13" s="139"/>
+      <c r="M13" s="132"/>
+      <c r="N13" s="139"/>
+      <c r="O13" s="139"/>
       <c r="P13" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="Q13" s="165"/>
-      <c r="R13" s="165"/>
-      <c r="S13" s="166"/>
+      <c r="Q13" s="145"/>
+      <c r="R13" s="145"/>
+      <c r="S13" s="158"/>
       <c r="T13" s="99"/>
       <c r="U13" s="100"/>
       <c r="V13" s="101" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="15" customHeight="1" thickBot="1">
       <c r="B14" s="91"/>
       <c r="C14" s="91"/>
-      <c r="D14" s="170"/>
-      <c r="E14" s="170"/>
-      <c r="F14" s="170"/>
+      <c r="D14" s="162"/>
+      <c r="E14" s="162"/>
+      <c r="F14" s="162"/>
       <c r="G14" s="91"/>
       <c r="H14" s="91"/>
       <c r="I14" s="91"/>
       <c r="J14" s="91"/>
       <c r="K14" s="92"/>
       <c r="L14" s="90"/>
-      <c r="M14" s="179"/>
+      <c r="M14" s="132"/>
       <c r="N14" s="89">
         <f>O14*Q14</f>
         <v>0</v>
@@ -2404,32 +2399,32 @@
       <c r="P14" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="Q14" s="171"/>
-      <c r="R14" s="171"/>
-      <c r="S14" s="172"/>
-      <c r="T14" s="173" t="s">
+      <c r="Q14" s="152"/>
+      <c r="R14" s="152"/>
+      <c r="S14" s="153"/>
+      <c r="T14" s="163" t="s">
         <v>49</v>
       </c>
-      <c r="U14" s="174"/>
-      <c r="V14" s="175"/>
-    </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="140"/>
-      <c r="C15" s="140"/>
-      <c r="D15" s="140"/>
-      <c r="E15" s="128" t="s">
+      <c r="U14" s="164"/>
+      <c r="V14" s="165"/>
+    </row>
+    <row r="15" spans="1:22" ht="15" customHeight="1" thickBot="1">
+      <c r="B15" s="166"/>
+      <c r="C15" s="166"/>
+      <c r="D15" s="166"/>
+      <c r="E15" s="169" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="140"/>
-      <c r="G15" s="140"/>
-      <c r="H15" s="140"/>
-      <c r="I15" s="140"/>
-      <c r="J15" s="128" t="s">
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="169" t="s">
         <v>51</v>
       </c>
       <c r="K15" s="92"/>
       <c r="L15" s="90"/>
-      <c r="M15" s="179"/>
+      <c r="M15" s="132"/>
       <c r="N15" s="90">
         <f>SUM(N14,N12,N11,N10,N8)</f>
         <v>0</v>
@@ -2439,67 +2434,67 @@
       </c>
       <c r="P15" s="62"/>
     </row>
-    <row r="16" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="140"/>
-      <c r="C16" s="140"/>
-      <c r="D16" s="140"/>
-      <c r="E16" s="128"/>
-      <c r="F16" s="140"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="140"/>
-      <c r="I16" s="140"/>
-      <c r="J16" s="128"/>
+    <row r="16" spans="1:22" ht="11.25" customHeight="1" thickBot="1">
+      <c r="B16" s="166"/>
+      <c r="C16" s="166"/>
+      <c r="D16" s="166"/>
+      <c r="E16" s="169"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="169"/>
       <c r="K16" s="92"/>
       <c r="L16" s="108"/>
-      <c r="M16" s="179"/>
-      <c r="T16" s="157" t="s">
+      <c r="M16" s="132"/>
+      <c r="T16" s="170" t="s">
         <v>53</v>
       </c>
-      <c r="U16" s="157"/>
-      <c r="V16" s="157"/>
-    </row>
-    <row r="17" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="140"/>
-      <c r="C17" s="140"/>
-      <c r="D17" s="140"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="152" t="s">
+      <c r="U16" s="170"/>
+      <c r="V16" s="170"/>
+    </row>
+    <row r="17" spans="1:22" ht="16.5" thickBot="1">
+      <c r="B17" s="166"/>
+      <c r="C17" s="166"/>
+      <c r="D17" s="166"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="168" t="s">
         <v>94</v>
       </c>
-      <c r="I17" s="152"/>
-      <c r="J17" s="152"/>
+      <c r="I17" s="168"/>
+      <c r="J17" s="168"/>
       <c r="K17" s="92"/>
-      <c r="M17" s="179"/>
+      <c r="M17" s="132"/>
       <c r="N17" s="63" t="s">
         <v>36</v>
       </c>
       <c r="O17" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="P17" s="153" t="s">
+      <c r="P17" s="174" t="s">
         <v>54</v>
       </c>
-      <c r="Q17" s="153"/>
-      <c r="R17" s="153"/>
-      <c r="S17" s="153"/>
-      <c r="T17" s="154" t="s">
+      <c r="Q17" s="174"/>
+      <c r="R17" s="174"/>
+      <c r="S17" s="174"/>
+      <c r="T17" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="U17" s="155"/>
-      <c r="V17" s="156"/>
-    </row>
-    <row r="18" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="140"/>
-      <c r="C18" s="140"/>
-      <c r="D18" s="140"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="152"/>
-      <c r="I18" s="152"/>
-      <c r="J18" s="152"/>
+      <c r="U17" s="136"/>
+      <c r="V17" s="137"/>
+    </row>
+    <row r="18" spans="1:22" ht="15" customHeight="1" thickBot="1">
+      <c r="B18" s="166"/>
+      <c r="C18" s="166"/>
+      <c r="D18" s="166"/>
+      <c r="E18" s="166"/>
+      <c r="F18" s="166"/>
+      <c r="G18" s="166"/>
+      <c r="H18" s="168"/>
+      <c r="I18" s="168"/>
+      <c r="J18" s="168"/>
       <c r="K18" s="84" t="s">
         <v>56</v>
       </c>
@@ -2514,25 +2509,25 @@
       <c r="S18" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="T18" s="143" t="s">
+      <c r="T18" s="173" t="s">
         <v>57</v>
       </c>
-      <c r="U18" s="143"/>
-      <c r="V18" s="143"/>
-    </row>
-    <row r="19" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="140"/>
-      <c r="B19" s="140"/>
-      <c r="C19" s="140"/>
-      <c r="D19" s="151" t="s">
+      <c r="U18" s="173"/>
+      <c r="V18" s="173"/>
+    </row>
+    <row r="19" spans="1:22" ht="15" customHeight="1" thickBot="1">
+      <c r="A19" s="166"/>
+      <c r="B19" s="166"/>
+      <c r="C19" s="166"/>
+      <c r="D19" s="167" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="151"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="140"/>
-      <c r="H19" s="140"/>
-      <c r="I19" s="140"/>
-      <c r="J19" s="128" t="s">
+      <c r="E19" s="167"/>
+      <c r="F19" s="166"/>
+      <c r="G19" s="166"/>
+      <c r="H19" s="166"/>
+      <c r="I19" s="166"/>
+      <c r="J19" s="169" t="s">
         <v>59</v>
       </c>
       <c r="K19" s="84"/>
@@ -2545,23 +2540,23 @@
       <c r="S19" s="104" t="s">
         <v>93</v>
       </c>
-      <c r="T19" s="143" t="s">
+      <c r="T19" s="173" t="s">
         <v>60</v>
       </c>
-      <c r="U19" s="143"/>
-      <c r="V19" s="143"/>
-    </row>
-    <row r="20" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="140"/>
-      <c r="B20" s="140"/>
-      <c r="C20" s="140"/>
-      <c r="D20" s="151"/>
-      <c r="E20" s="151"/>
-      <c r="F20" s="140"/>
-      <c r="G20" s="140"/>
-      <c r="H20" s="140"/>
-      <c r="I20" s="140"/>
-      <c r="J20" s="128"/>
+      <c r="U19" s="173"/>
+      <c r="V19" s="173"/>
+    </row>
+    <row r="20" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A20" s="166"/>
+      <c r="B20" s="166"/>
+      <c r="C20" s="166"/>
+      <c r="D20" s="167"/>
+      <c r="E20" s="167"/>
+      <c r="F20" s="166"/>
+      <c r="G20" s="166"/>
+      <c r="H20" s="166"/>
+      <c r="I20" s="166"/>
+      <c r="J20" s="169"/>
       <c r="K20" s="92"/>
       <c r="L20" s="90"/>
       <c r="N20" s="90"/>
@@ -2572,13 +2567,13 @@
       <c r="S20" s="103" t="s">
         <v>96</v>
       </c>
-      <c r="T20" s="143" t="s">
+      <c r="T20" s="173" t="s">
         <v>61</v>
       </c>
-      <c r="U20" s="143"/>
-      <c r="V20" s="143"/>
-    </row>
-    <row r="21" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U20" s="173"/>
+      <c r="V20" s="173"/>
+    </row>
+    <row r="21" spans="1:22" ht="16.5" thickBot="1">
       <c r="B21" s="91"/>
       <c r="C21" s="91"/>
       <c r="D21" s="91"/>
@@ -2598,20 +2593,20 @@
       <c r="S21" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="T21" s="143" t="s">
+      <c r="T21" s="173" t="s">
         <v>63</v>
       </c>
-      <c r="U21" s="143"/>
-      <c r="V21" s="143"/>
-    </row>
-    <row r="22" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U21" s="173"/>
+      <c r="V21" s="173"/>
+    </row>
+    <row r="22" spans="1:22" ht="15" customHeight="1" thickBot="1">
       <c r="B22" s="91"/>
       <c r="C22" s="91"/>
       <c r="D22" s="91"/>
-      <c r="E22" s="144" t="s">
+      <c r="E22" s="175" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="145"/>
+      <c r="F22" s="148"/>
       <c r="G22" s="91"/>
       <c r="H22" s="91"/>
       <c r="I22" s="91"/>
@@ -2620,20 +2615,20 @@
       <c r="L22" s="90"/>
       <c r="N22" s="90"/>
       <c r="O22" s="95"/>
-      <c r="P22" s="148"/>
-      <c r="Q22" s="148"/>
-      <c r="R22" s="148"/>
-      <c r="S22" s="148"/>
-      <c r="T22" s="149"/>
-      <c r="U22" s="149"/>
-      <c r="V22" s="149"/>
-    </row>
-    <row r="23" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P22" s="140"/>
+      <c r="Q22" s="140"/>
+      <c r="R22" s="140"/>
+      <c r="S22" s="140"/>
+      <c r="T22" s="176"/>
+      <c r="U22" s="176"/>
+      <c r="V22" s="176"/>
+    </row>
+    <row r="23" spans="1:22" ht="15" customHeight="1" thickBot="1">
       <c r="B23" s="91"/>
       <c r="C23" s="91"/>
       <c r="D23" s="91"/>
-      <c r="E23" s="146"/>
-      <c r="F23" s="147"/>
+      <c r="E23" s="149"/>
+      <c r="F23" s="151"/>
       <c r="G23" s="91"/>
       <c r="H23" s="91"/>
       <c r="I23" s="105"/>
@@ -2644,296 +2639,296 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="140" t="s">
+    <row r="24" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A24" s="166" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="140"/>
-      <c r="C24" s="140"/>
-      <c r="D24" s="140"/>
-      <c r="E24" s="135" t="s">
+      <c r="B24" s="166"/>
+      <c r="C24" s="166"/>
+      <c r="D24" s="166"/>
+      <c r="E24" s="129" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="140" t="s">
+      <c r="F24" s="166" t="s">
         <v>91</v>
       </c>
-      <c r="G24" s="140"/>
-      <c r="H24" s="135" t="s">
+      <c r="G24" s="166"/>
+      <c r="H24" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="I24" s="135"/>
-      <c r="J24" s="135"/>
+      <c r="I24" s="129"/>
+      <c r="J24" s="129"/>
       <c r="K24" s="92"/>
     </row>
-    <row r="25" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="140"/>
-      <c r="B25" s="140"/>
-      <c r="C25" s="140"/>
-      <c r="D25" s="140"/>
-      <c r="E25" s="135"/>
-      <c r="F25" s="140"/>
-      <c r="G25" s="140"/>
-      <c r="H25" s="135"/>
-      <c r="I25" s="135"/>
-      <c r="J25" s="135"/>
+    <row r="25" spans="1:22" ht="15" customHeight="1" thickBot="1">
+      <c r="A25" s="166"/>
+      <c r="B25" s="166"/>
+      <c r="C25" s="166"/>
+      <c r="D25" s="166"/>
+      <c r="E25" s="129"/>
+      <c r="F25" s="166"/>
+      <c r="G25" s="166"/>
+      <c r="H25" s="129"/>
+      <c r="I25" s="129"/>
+      <c r="J25" s="129"/>
       <c r="K25" s="92"/>
       <c r="L25" s="90"/>
       <c r="N25" s="90"/>
       <c r="O25" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="P25" s="150" t="s">
+      <c r="P25" s="178" t="s">
         <v>69</v>
       </c>
-      <c r="Q25" s="150"/>
-      <c r="R25" s="150"/>
-      <c r="S25" s="150"/>
-      <c r="T25" s="150"/>
-      <c r="U25" s="150"/>
-    </row>
-    <row r="26" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="126"/>
-      <c r="C26" s="140" t="s">
+      <c r="Q25" s="178"/>
+      <c r="R25" s="178"/>
+      <c r="S25" s="178"/>
+      <c r="T25" s="178"/>
+      <c r="U25" s="178"/>
+    </row>
+    <row r="26" spans="1:22" ht="11.25" customHeight="1" thickBot="1">
+      <c r="B26" s="171"/>
+      <c r="C26" s="166" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="140"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
-      <c r="G26" s="140"/>
-      <c r="H26" s="140"/>
-      <c r="I26" s="140"/>
-      <c r="J26" s="135" t="s">
+      <c r="D26" s="166"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="166"/>
+      <c r="H26" s="166"/>
+      <c r="I26" s="166"/>
+      <c r="J26" s="129" t="s">
         <v>70</v>
       </c>
       <c r="K26" s="92"/>
     </row>
-    <row r="27" spans="1:22" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="126"/>
-      <c r="C27" s="140"/>
-      <c r="D27" s="140"/>
-      <c r="E27" s="140"/>
-      <c r="F27" s="140"/>
-      <c r="G27" s="140"/>
-      <c r="H27" s="140"/>
-      <c r="I27" s="140"/>
-      <c r="J27" s="135"/>
+    <row r="27" spans="1:22" ht="14.25" customHeight="1" thickBot="1">
+      <c r="B27" s="171"/>
+      <c r="C27" s="166"/>
+      <c r="D27" s="166"/>
+      <c r="E27" s="166"/>
+      <c r="F27" s="166"/>
+      <c r="G27" s="166"/>
+      <c r="H27" s="166"/>
+      <c r="I27" s="166"/>
+      <c r="J27" s="129"/>
       <c r="K27" s="92"/>
       <c r="L27" s="90"/>
       <c r="N27" s="90"/>
-      <c r="P27" s="132" t="s">
+      <c r="P27" s="172" t="s">
         <v>71</v>
       </c>
-      <c r="Q27" s="132"/>
-      <c r="R27" s="132"/>
-      <c r="S27" s="132"/>
-      <c r="T27" s="132"/>
-      <c r="U27" s="127" t="s">
+      <c r="Q27" s="172"/>
+      <c r="R27" s="172"/>
+      <c r="S27" s="172"/>
+      <c r="T27" s="172"/>
+      <c r="U27" s="177" t="s">
         <v>72</v>
       </c>
-      <c r="V27" s="127"/>
-    </row>
-    <row r="28" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="127" t="s">
+      <c r="V27" s="177"/>
+    </row>
+    <row r="28" spans="1:22" ht="19.5" thickBot="1">
+      <c r="A28" s="177" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="127"/>
-      <c r="C28" s="128" t="s">
+      <c r="B28" s="177"/>
+      <c r="C28" s="169" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="128"/>
-      <c r="E28" s="128"/>
-      <c r="F28" s="128"/>
-      <c r="G28" s="128"/>
-      <c r="H28" s="128"/>
-      <c r="I28" s="128"/>
-      <c r="J28" s="128"/>
+      <c r="D28" s="169"/>
+      <c r="E28" s="169"/>
+      <c r="F28" s="169"/>
+      <c r="G28" s="169"/>
+      <c r="H28" s="169"/>
+      <c r="I28" s="169"/>
+      <c r="J28" s="169"/>
       <c r="K28" s="92"/>
-      <c r="U28" s="127" t="s">
+      <c r="U28" s="177" t="s">
         <v>74</v>
       </c>
-      <c r="V28" s="127"/>
-    </row>
-    <row r="29" spans="1:22" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="127"/>
-      <c r="B29" s="127"/>
-      <c r="C29" s="128"/>
-      <c r="D29" s="128"/>
-      <c r="E29" s="128"/>
-      <c r="F29" s="128"/>
-      <c r="G29" s="128"/>
-      <c r="H29" s="128"/>
-      <c r="I29" s="128"/>
-      <c r="J29" s="128"/>
+      <c r="V28" s="177"/>
+    </row>
+    <row r="29" spans="1:22" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A29" s="177"/>
+      <c r="B29" s="177"/>
+      <c r="C29" s="169"/>
+      <c r="D29" s="169"/>
+      <c r="E29" s="169"/>
+      <c r="F29" s="169"/>
+      <c r="G29" s="169"/>
+      <c r="H29" s="169"/>
+      <c r="I29" s="169"/>
+      <c r="J29" s="169"/>
       <c r="K29" s="92"/>
       <c r="L29" s="90"/>
       <c r="N29" s="90"/>
-      <c r="P29" s="132" t="s">
+      <c r="P29" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="Q29" s="132"/>
-      <c r="R29" s="132"/>
-      <c r="S29" s="132"/>
-      <c r="T29" s="132"/>
-    </row>
-    <row r="30" spans="1:22" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E30" s="137" t="s">
+      <c r="Q29" s="172"/>
+      <c r="R29" s="172"/>
+      <c r="S29" s="172"/>
+      <c r="T29" s="172"/>
+    </row>
+    <row r="30" spans="1:22" ht="16.5" customHeight="1" thickBot="1">
+      <c r="E30" s="181" t="s">
         <v>76</v>
       </c>
-      <c r="F30" s="138"/>
+      <c r="F30" s="182"/>
       <c r="K30" s="92"/>
     </row>
-    <row r="31" spans="1:22" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="139"/>
-      <c r="C31" s="140"/>
-      <c r="D31" s="140"/>
-      <c r="E31" s="140"/>
-      <c r="F31" s="140"/>
-      <c r="G31" s="140"/>
-      <c r="H31" s="140"/>
-      <c r="I31" s="135" t="s">
+    <row r="31" spans="1:22" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B31" s="183"/>
+      <c r="C31" s="166"/>
+      <c r="D31" s="166"/>
+      <c r="E31" s="166"/>
+      <c r="F31" s="166"/>
+      <c r="G31" s="166"/>
+      <c r="H31" s="166"/>
+      <c r="I31" s="129" t="s">
         <v>77</v>
       </c>
-      <c r="J31" s="135"/>
+      <c r="J31" s="129"/>
       <c r="K31" s="92"/>
       <c r="L31" s="90"/>
       <c r="N31" s="109"/>
-      <c r="O31" s="129" t="s">
+      <c r="O31" s="186" t="s">
         <v>78</v>
       </c>
-      <c r="P31" s="130"/>
-    </row>
-    <row r="32" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="140"/>
-      <c r="C32" s="140"/>
-      <c r="D32" s="140"/>
-      <c r="E32" s="140"/>
-      <c r="F32" s="140"/>
-      <c r="G32" s="140"/>
-      <c r="H32" s="140"/>
-      <c r="I32" s="135"/>
-      <c r="J32" s="135"/>
+      <c r="P31" s="187"/>
+    </row>
+    <row r="32" spans="1:22" ht="14.25" customHeight="1">
+      <c r="B32" s="166"/>
+      <c r="C32" s="166"/>
+      <c r="D32" s="166"/>
+      <c r="E32" s="166"/>
+      <c r="F32" s="166"/>
+      <c r="G32" s="166"/>
+      <c r="H32" s="166"/>
+      <c r="I32" s="129"/>
+      <c r="J32" s="129"/>
       <c r="K32" s="92"/>
     </row>
-    <row r="33" spans="2:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="127"/>
-      <c r="C33" s="127"/>
-      <c r="D33" s="127"/>
-      <c r="E33" s="127"/>
-      <c r="F33" s="127"/>
-      <c r="G33" s="127"/>
-      <c r="H33" s="128" t="s">
+    <row r="33" spans="2:22" ht="16.5" customHeight="1">
+      <c r="B33" s="177"/>
+      <c r="C33" s="177"/>
+      <c r="D33" s="177"/>
+      <c r="E33" s="177"/>
+      <c r="F33" s="177"/>
+      <c r="G33" s="177"/>
+      <c r="H33" s="169" t="s">
         <v>79</v>
       </c>
-      <c r="I33" s="128"/>
-      <c r="J33" s="128"/>
+      <c r="I33" s="169"/>
+      <c r="J33" s="169"/>
       <c r="K33" s="92"/>
     </row>
-    <row r="34" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="127"/>
-      <c r="C34" s="127"/>
-      <c r="D34" s="127"/>
-      <c r="E34" s="127"/>
-      <c r="F34" s="127"/>
-      <c r="G34" s="127"/>
-      <c r="H34" s="128"/>
-      <c r="I34" s="128"/>
-      <c r="J34" s="128"/>
+    <row r="34" spans="2:22" ht="15.75" customHeight="1">
+      <c r="B34" s="177"/>
+      <c r="C34" s="177"/>
+      <c r="D34" s="177"/>
+      <c r="E34" s="177"/>
+      <c r="F34" s="177"/>
+      <c r="G34" s="177"/>
+      <c r="H34" s="169"/>
+      <c r="I34" s="169"/>
+      <c r="J34" s="169"/>
       <c r="L34" s="108"/>
-      <c r="O34" s="131" t="s">
+      <c r="O34" s="188" t="s">
         <v>80</v>
       </c>
-      <c r="P34" s="131"/>
-      <c r="Q34" s="131"/>
-      <c r="R34" s="131"/>
-      <c r="S34" s="131"/>
-      <c r="T34" s="131"/>
-      <c r="U34" s="131"/>
-      <c r="V34" s="131"/>
-    </row>
-    <row r="35" spans="2:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="127" t="s">
+      <c r="P34" s="188"/>
+      <c r="Q34" s="188"/>
+      <c r="R34" s="188"/>
+      <c r="S34" s="188"/>
+      <c r="T34" s="188"/>
+      <c r="U34" s="188"/>
+      <c r="V34" s="188"/>
+    </row>
+    <row r="35" spans="2:22" ht="11.25" customHeight="1">
+      <c r="B35" s="177" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="127"/>
-      <c r="D35" s="127"/>
-      <c r="E35" s="127"/>
-      <c r="F35" s="127"/>
-      <c r="G35" s="127"/>
-      <c r="H35" s="141" t="s">
+      <c r="C35" s="177"/>
+      <c r="D35" s="177"/>
+      <c r="E35" s="177"/>
+      <c r="F35" s="177"/>
+      <c r="G35" s="177"/>
+      <c r="H35" s="184" t="s">
         <v>81</v>
       </c>
-      <c r="I35" s="141"/>
-      <c r="J35" s="141"/>
-    </row>
-    <row r="36" spans="2:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="127"/>
-      <c r="C36" s="127"/>
-      <c r="D36" s="127"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="127"/>
-      <c r="G36" s="127"/>
-      <c r="H36" s="141"/>
-      <c r="I36" s="141"/>
-      <c r="J36" s="141"/>
-      <c r="L36" s="127" t="e">
+      <c r="I35" s="184"/>
+      <c r="J35" s="184"/>
+    </row>
+    <row r="36" spans="2:22" ht="16.5" customHeight="1">
+      <c r="B36" s="177"/>
+      <c r="C36" s="177"/>
+      <c r="D36" s="177"/>
+      <c r="E36" s="177"/>
+      <c r="F36" s="177"/>
+      <c r="G36" s="177"/>
+      <c r="H36" s="184"/>
+      <c r="I36" s="184"/>
+      <c r="J36" s="184"/>
+      <c r="L36" s="177" t="e">
         <f ca="1">[1]!ChangeThisNumber(N31)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M36" s="127"/>
-      <c r="N36" s="127"/>
-      <c r="O36" s="127"/>
-      <c r="P36" s="127"/>
-      <c r="Q36" s="127"/>
-      <c r="R36" s="127"/>
-      <c r="S36" s="127"/>
-      <c r="T36" s="127"/>
-      <c r="U36" s="127"/>
+      <c r="M36" s="177"/>
+      <c r="N36" s="177"/>
+      <c r="O36" s="177"/>
+      <c r="P36" s="177"/>
+      <c r="Q36" s="177"/>
+      <c r="R36" s="177"/>
+      <c r="S36" s="177"/>
+      <c r="T36" s="177"/>
+      <c r="U36" s="177"/>
       <c r="V36" s="107" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="2:22" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="127"/>
-      <c r="C37" s="127"/>
-      <c r="D37" s="127"/>
-      <c r="E37" s="127"/>
-      <c r="F37" s="135" t="s">
+    <row r="37" spans="2:22" ht="18.75">
+      <c r="B37" s="177"/>
+      <c r="C37" s="177"/>
+      <c r="D37" s="177"/>
+      <c r="E37" s="177"/>
+      <c r="F37" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="G37" s="135"/>
-      <c r="H37" s="135"/>
-      <c r="I37" s="135"/>
-      <c r="J37" s="135"/>
+      <c r="G37" s="129"/>
+      <c r="H37" s="129"/>
+      <c r="I37" s="129"/>
+      <c r="J37" s="129"/>
       <c r="K37" s="64" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="2:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:22" ht="13.5" customHeight="1">
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
-      <c r="L38" s="136"/>
-      <c r="M38" s="136"/>
-      <c r="N38" s="136"/>
+      <c r="L38" s="180"/>
+      <c r="M38" s="180"/>
+      <c r="N38" s="180"/>
       <c r="O38" s="107" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="134"/>
-      <c r="C39" s="134"/>
-      <c r="D39" s="134"/>
-      <c r="E39" s="134"/>
+    <row r="39" spans="2:22" ht="15" customHeight="1">
+      <c r="B39" s="128"/>
+      <c r="C39" s="128"/>
+      <c r="D39" s="128"/>
+      <c r="E39" s="128"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="135" t="s">
+      <c r="G39" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="H39" s="135"/>
-      <c r="I39" s="135"/>
-      <c r="J39" s="135"/>
-    </row>
-    <row r="40" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="129"/>
+      <c r="I39" s="129"/>
+      <c r="J39" s="129"/>
+    </row>
+    <row r="40" spans="2:22" ht="15" customHeight="1">
       <c r="B40" s="88"/>
       <c r="C40" s="88"/>
       <c r="D40" s="88"/>
@@ -2943,49 +2938,116 @@
       <c r="H40" s="88"/>
       <c r="I40" s="88"/>
       <c r="J40" s="88"/>
-      <c r="O40" s="142" t="s">
+      <c r="O40" s="185" t="s">
         <v>86</v>
       </c>
-      <c r="P40" s="142"/>
-      <c r="T40" s="126" t="s">
+      <c r="P40" s="185"/>
+      <c r="T40" s="171" t="s">
         <v>87</v>
       </c>
-      <c r="U40" s="126"/>
-    </row>
-    <row r="41" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O41" s="126" t="s">
+      <c r="U40" s="171"/>
+    </row>
+    <row r="41" spans="2:22" ht="15" customHeight="1">
+      <c r="O41" s="171" t="s">
         <v>88</v>
       </c>
-      <c r="P41" s="127"/>
-      <c r="T41" s="126" t="s">
+      <c r="P41" s="177"/>
+      <c r="T41" s="171" t="s">
         <v>89</v>
       </c>
-      <c r="U41" s="127"/>
-    </row>
-    <row r="42" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H43" s="133" t="s">
+      <c r="U41" s="177"/>
+    </row>
+    <row r="42" spans="2:22" ht="15" customHeight="1"/>
+    <row r="43" spans="2:22" ht="15" customHeight="1">
+      <c r="H43" s="179" t="s">
         <v>90</v>
       </c>
-      <c r="I43" s="133"/>
-      <c r="J43" s="133"/>
-    </row>
-    <row r="44" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I43" s="179"/>
+      <c r="J43" s="179"/>
+    </row>
+    <row r="44" spans="2:22" ht="15" customHeight="1">
       <c r="I44" s="65"/>
       <c r="J44" s="65"/>
     </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:22">
       <c r="E45" s="87"/>
       <c r="F45" s="87"/>
     </row>
-    <row r="46" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:22" ht="15" customHeight="1">
       <c r="E46" s="87"/>
       <c r="F46" s="87"/>
     </row>
-    <row r="47" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:22" ht="15" customHeight="1"/>
+    <row r="48" spans="2:22" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="83">
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="A28:B29"/>
+    <mergeCell ref="C28:J29"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="O34:V34"/>
+    <mergeCell ref="P29:T29"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="L38:N38"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B31:H32"/>
+    <mergeCell ref="I31:J32"/>
+    <mergeCell ref="B33:G34"/>
+    <mergeCell ref="H33:J34"/>
+    <mergeCell ref="B35:G36"/>
+    <mergeCell ref="H35:J36"/>
+    <mergeCell ref="L36:U36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:J37"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="T40:U40"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="P22:S22"/>
+    <mergeCell ref="T22:V22"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="H24:J25"/>
+    <mergeCell ref="P25:U25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="P27:T27"/>
+    <mergeCell ref="T18:V18"/>
+    <mergeCell ref="A19:C20"/>
+    <mergeCell ref="D19:E20"/>
+    <mergeCell ref="F19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="T19:V19"/>
+    <mergeCell ref="T20:V20"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="P17:S17"/>
+    <mergeCell ref="T17:V17"/>
+    <mergeCell ref="A24:D25"/>
+    <mergeCell ref="B15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="Q12:S13"/>
+    <mergeCell ref="T12:V12"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="A12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="N12:N13"/>
     <mergeCell ref="P3:S4"/>
     <mergeCell ref="C4:H5"/>
     <mergeCell ref="T5:V6"/>
@@ -3002,73 +3064,6 @@
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="T10:U10"/>
     <mergeCell ref="P11:S11"/>
-    <mergeCell ref="T11:V11"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="Q12:S13"/>
-    <mergeCell ref="T12:V12"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="T14:V14"/>
-    <mergeCell ref="A12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="B15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="T16:V16"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="P27:T27"/>
-    <mergeCell ref="T18:V18"/>
-    <mergeCell ref="A19:C20"/>
-    <mergeCell ref="D19:E20"/>
-    <mergeCell ref="F19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="T19:V19"/>
-    <mergeCell ref="T20:V20"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="P17:S17"/>
-    <mergeCell ref="T17:V17"/>
-    <mergeCell ref="A24:D25"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="P22:S22"/>
-    <mergeCell ref="T22:V22"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:G25"/>
-    <mergeCell ref="H24:J25"/>
-    <mergeCell ref="P25:U25"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="L38:N38"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B31:H32"/>
-    <mergeCell ref="I31:J32"/>
-    <mergeCell ref="B33:G34"/>
-    <mergeCell ref="H33:J34"/>
-    <mergeCell ref="B35:G36"/>
-    <mergeCell ref="H35:J36"/>
-    <mergeCell ref="L36:U36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:J37"/>
-    <mergeCell ref="O40:P40"/>
-    <mergeCell ref="T40:U40"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="C28:J29"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="O34:V34"/>
-    <mergeCell ref="P29:T29"/>
-    <mergeCell ref="U28:V28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" verticalDpi="720" r:id="rId1"/>
@@ -3077,14 +3072,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="10" customWidth="1" collapsed="1"/>
@@ -3106,7 +3101,7 @@
     <col min="20" max="20" width="23.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -3117,7 +3112,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="18.75">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -3133,7 +3128,7 @@
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15.75" customHeight="1" thickBot="1">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -3147,123 +3142,123 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:21" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="194" t="s">
+    <row r="4" spans="1:21" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A4" s="204" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="195"/>
-      <c r="C4" s="144" t="s">
+      <c r="B4" s="205"/>
+      <c r="C4" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="200"/>
-      <c r="E4" s="200"/>
-      <c r="F4" s="200"/>
+      <c r="D4" s="210"/>
+      <c r="E4" s="210"/>
+      <c r="F4" s="210"/>
       <c r="G4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="144" t="s">
+      <c r="H4" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="187"/>
-      <c r="J4" s="145"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="148"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="201" t="s">
+      <c r="L4" s="211" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="221" t="s">
+      <c r="M4" s="191" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="222"/>
-      <c r="O4" s="215" t="s">
+      <c r="N4" s="192"/>
+      <c r="O4" s="223" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="216"/>
-      <c r="Q4" s="203" t="s">
+      <c r="P4" s="224"/>
+      <c r="Q4" s="213" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="204"/>
-      <c r="S4" s="205"/>
+      <c r="R4" s="214"/>
+      <c r="S4" s="215"/>
       <c r="T4" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="196"/>
-      <c r="B5" s="197"/>
-      <c r="C5" s="206" t="s">
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A5" s="206"/>
+      <c r="B5" s="207"/>
+      <c r="C5" s="216" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="207"/>
-      <c r="E5" s="207"/>
-      <c r="F5" s="208"/>
+      <c r="D5" s="217"/>
+      <c r="E5" s="217"/>
+      <c r="F5" s="218"/>
       <c r="G5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="209" t="s">
+      <c r="H5" s="219" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="209" t="s">
+      <c r="I5" s="219" t="s">
         <v>12</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K5" s="5"/>
-      <c r="L5" s="202"/>
-      <c r="M5" s="217" t="s">
+      <c r="L5" s="212"/>
+      <c r="M5" s="193" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="218"/>
-      <c r="O5" s="217" t="s">
+      <c r="N5" s="194"/>
+      <c r="O5" s="193" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="218"/>
-      <c r="Q5" s="190"/>
-      <c r="R5" s="191"/>
-      <c r="S5" s="192"/>
+      <c r="P5" s="194"/>
+      <c r="Q5" s="200"/>
+      <c r="R5" s="201"/>
+      <c r="S5" s="202"/>
       <c r="T5" s="10"/>
     </row>
-    <row r="6" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="196"/>
-      <c r="B6" s="197"/>
-      <c r="C6" s="211" t="s">
+    <row r="6" spans="1:21" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A6" s="206"/>
+      <c r="B6" s="207"/>
+      <c r="C6" s="221" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="212"/>
-      <c r="E6" s="213" t="s">
+      <c r="D6" s="222"/>
+      <c r="E6" s="197" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="214"/>
+      <c r="F6" s="198"/>
       <c r="G6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="210"/>
-      <c r="I6" s="210"/>
+      <c r="H6" s="220"/>
+      <c r="I6" s="220"/>
       <c r="J6" s="11" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="12"/>
-      <c r="L6" s="189" t="s">
+      <c r="L6" s="199" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="223" t="s">
+      <c r="M6" s="195" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="224"/>
-      <c r="O6" s="217" t="s">
+      <c r="N6" s="196"/>
+      <c r="O6" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="218"/>
-      <c r="Q6" s="190" t="s">
+      <c r="P6" s="194"/>
+      <c r="Q6" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="191"/>
-      <c r="S6" s="192"/>
+      <c r="R6" s="201"/>
+      <c r="S6" s="202"/>
       <c r="T6" s="10"/>
     </row>
-    <row r="7" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="196"/>
-      <c r="B7" s="197"/>
+    <row r="7" spans="1:21" ht="16.5" customHeight="1">
+      <c r="A7" s="206"/>
+      <c r="B7" s="207"/>
       <c r="C7" s="13" t="s">
         <v>23</v>
       </c>
@@ -3281,19 +3276,19 @@
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
       <c r="K7" s="12"/>
-      <c r="L7" s="189"/>
+      <c r="L7" s="199"/>
       <c r="M7" s="74"/>
       <c r="N7" s="75"/>
       <c r="O7" s="76"/>
       <c r="P7" s="48"/>
-      <c r="Q7" s="190"/>
-      <c r="R7" s="191"/>
-      <c r="S7" s="192"/>
+      <c r="Q7" s="200"/>
+      <c r="R7" s="201"/>
+      <c r="S7" s="202"/>
       <c r="T7" s="10"/>
     </row>
-    <row r="8" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="198"/>
-      <c r="B8" s="199"/>
+    <row r="8" spans="1:21" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A8" s="208"/>
+      <c r="B8" s="209"/>
       <c r="C8" s="18">
         <v>13</v>
       </c>
@@ -3322,14 +3317,14 @@
       <c r="L8" s="20">
         <v>5</v>
       </c>
-      <c r="M8" s="213">
+      <c r="M8" s="197">
         <v>4</v>
       </c>
-      <c r="N8" s="214"/>
-      <c r="O8" s="219">
+      <c r="N8" s="198"/>
+      <c r="O8" s="189">
         <v>3</v>
       </c>
-      <c r="P8" s="220"/>
+      <c r="P8" s="190"/>
       <c r="Q8" s="23"/>
       <c r="R8" s="24">
         <v>2</v>
@@ -3339,7 +3334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.75" customHeight="1">
       <c r="A9" s="27"/>
       <c r="B9" s="28"/>
       <c r="C9" s="112"/>
@@ -3361,7 +3356,7 @@
       <c r="S9" s="125"/>
       <c r="T9" s="119"/>
     </row>
-    <row r="10" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="16.5" customHeight="1">
       <c r="A10" s="30"/>
       <c r="B10" s="31" t="s">
         <v>91</v>
@@ -3386,7 +3381,7 @@
       <c r="S10" s="72"/>
       <c r="T10" s="66"/>
     </row>
-    <row r="11" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="18.75">
       <c r="A11" s="30"/>
       <c r="B11" s="34"/>
       <c r="C11" s="114"/>
@@ -3407,7 +3402,7 @@
       <c r="S11" s="72"/>
       <c r="T11" s="66"/>
     </row>
-    <row r="12" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="16.5" customHeight="1">
       <c r="A12" s="30"/>
       <c r="B12" s="34" t="s">
         <v>91</v>
@@ -3432,7 +3427,7 @@
       <c r="S12" s="72"/>
       <c r="T12" s="66"/>
     </row>
-    <row r="13" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="16.5" customHeight="1">
       <c r="A13" s="30"/>
       <c r="B13" s="34"/>
       <c r="C13" s="114"/>
@@ -3453,7 +3448,7 @@
       <c r="S13" s="72"/>
       <c r="T13" s="66"/>
     </row>
-    <row r="14" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="16.5" customHeight="1">
       <c r="A14" s="30"/>
       <c r="B14" s="34" t="s">
         <v>91</v>
@@ -3478,7 +3473,7 @@
       <c r="S14" s="72"/>
       <c r="T14" s="66"/>
     </row>
-    <row r="15" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="16.5" customHeight="1">
       <c r="A15" s="40"/>
       <c r="B15" s="41"/>
       <c r="C15" s="114"/>
@@ -3499,7 +3494,7 @@
       <c r="S15" s="72"/>
       <c r="T15" s="66"/>
     </row>
-    <row r="16" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="16.5" customHeight="1">
       <c r="A16" s="40"/>
       <c r="B16" s="41"/>
       <c r="C16" s="114"/>
@@ -3520,7 +3515,7 @@
       <c r="S16" s="72"/>
       <c r="T16" s="66"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="A17" s="30"/>
       <c r="B17" s="31"/>
       <c r="C17" s="114"/>
@@ -3541,7 +3536,7 @@
       <c r="S17" s="72"/>
       <c r="T17" s="66"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="A18" s="30"/>
       <c r="B18" s="31"/>
       <c r="C18" s="114"/>
@@ -3562,7 +3557,7 @@
       <c r="S18" s="72"/>
       <c r="T18" s="66"/>
     </row>
-    <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="15.75">
       <c r="A19" s="42"/>
       <c r="B19" s="33"/>
       <c r="C19" s="114"/>
@@ -3583,7 +3578,7 @@
       <c r="S19" s="72"/>
       <c r="T19" s="66"/>
     </row>
-    <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="15.75">
       <c r="A20" s="42"/>
       <c r="B20" s="33"/>
       <c r="C20" s="114"/>
@@ -3604,7 +3599,7 @@
       <c r="S20" s="72"/>
       <c r="T20" s="66"/>
     </row>
-    <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15.75">
       <c r="A21" s="42"/>
       <c r="B21" s="33"/>
       <c r="C21" s="114"/>
@@ -3625,7 +3620,7 @@
       <c r="S21" s="72"/>
       <c r="T21" s="66"/>
     </row>
-    <row r="22" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="15.75">
       <c r="A22" s="42"/>
       <c r="B22" s="33"/>
       <c r="C22" s="114"/>
@@ -3646,7 +3641,7 @@
       <c r="S22" s="72"/>
       <c r="T22" s="66"/>
     </row>
-    <row r="23" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="15.75">
       <c r="A23" s="42"/>
       <c r="B23" s="33"/>
       <c r="C23" s="114"/>
@@ -3667,7 +3662,7 @@
       <c r="S23" s="72"/>
       <c r="T23" s="66"/>
     </row>
-    <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="15.75">
       <c r="A24" s="42"/>
       <c r="B24" s="33"/>
       <c r="C24" s="114"/>
@@ -3688,7 +3683,7 @@
       <c r="S24" s="72"/>
       <c r="T24" s="66"/>
     </row>
-    <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="15.75">
       <c r="A25" s="42"/>
       <c r="B25" s="33"/>
       <c r="C25" s="114"/>
@@ -3709,7 +3704,7 @@
       <c r="S25" s="72"/>
       <c r="T25" s="66"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="A26" s="30"/>
       <c r="B26" s="48"/>
       <c r="C26" s="114"/>
@@ -3730,7 +3725,7 @@
       <c r="S26" s="72"/>
       <c r="T26" s="66"/>
     </row>
-    <row r="27" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="18.75">
       <c r="A27" s="30"/>
       <c r="B27" s="41"/>
       <c r="C27" s="114"/>
@@ -3751,7 +3746,7 @@
       <c r="S27" s="72"/>
       <c r="T27" s="66"/>
     </row>
-    <row r="28" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="18.75">
       <c r="A28" s="30"/>
       <c r="B28" s="37"/>
       <c r="C28" s="114"/>
@@ -3772,7 +3767,7 @@
       <c r="S28" s="72"/>
       <c r="T28" s="66"/>
     </row>
-    <row r="29" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="18.75">
       <c r="A29" s="30"/>
       <c r="B29" s="49"/>
       <c r="C29" s="114"/>
@@ -3793,7 +3788,7 @@
       <c r="S29" s="72"/>
       <c r="T29" s="66"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20">
       <c r="A30" s="30"/>
       <c r="B30" s="33"/>
       <c r="C30" s="114"/>
@@ -3814,7 +3809,7 @@
       <c r="S30" s="72"/>
       <c r="T30" s="66"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20">
       <c r="A31" s="30"/>
       <c r="B31" s="33"/>
       <c r="C31" s="114"/>
@@ -3835,7 +3830,7 @@
       <c r="S31" s="72"/>
       <c r="T31" s="66"/>
     </row>
-    <row r="32" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="18.75">
       <c r="A32" s="30"/>
       <c r="B32" s="33"/>
       <c r="C32" s="114"/>
@@ -3856,7 +3851,7 @@
       <c r="S32" s="72"/>
       <c r="T32" s="66"/>
     </row>
-    <row r="33" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="18.75">
       <c r="A33" s="30"/>
       <c r="B33" s="33"/>
       <c r="C33" s="114"/>
@@ -3877,7 +3872,7 @@
       <c r="S33" s="72"/>
       <c r="T33" s="66"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20">
       <c r="A34" s="30"/>
       <c r="B34" s="33"/>
       <c r="C34" s="114"/>
@@ -3898,7 +3893,7 @@
       <c r="S34" s="72"/>
       <c r="T34" s="66"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20">
       <c r="A35" s="30"/>
       <c r="B35" s="33"/>
       <c r="C35" s="114"/>
@@ -3919,7 +3914,7 @@
       <c r="S35" s="72"/>
       <c r="T35" s="66"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20">
       <c r="A36" s="30"/>
       <c r="B36" s="33"/>
       <c r="C36" s="114"/>
@@ -3940,7 +3935,7 @@
       <c r="S36" s="72"/>
       <c r="T36" s="66"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20">
       <c r="A37" s="30"/>
       <c r="B37" s="33"/>
       <c r="C37" s="114"/>
@@ -3961,7 +3956,7 @@
       <c r="S37" s="72"/>
       <c r="T37" s="66"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20">
       <c r="A38" s="30"/>
       <c r="B38" s="33"/>
       <c r="C38" s="114"/>
@@ -3982,7 +3977,7 @@
       <c r="S38" s="72"/>
       <c r="T38" s="66"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20">
       <c r="A39" s="30"/>
       <c r="B39" s="33"/>
       <c r="C39" s="114"/>
@@ -4003,7 +3998,7 @@
       <c r="S39" s="72"/>
       <c r="T39" s="66"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20">
       <c r="A40" s="30"/>
       <c r="B40" s="33"/>
       <c r="C40" s="114"/>
@@ -4024,7 +4019,7 @@
       <c r="S40" s="72"/>
       <c r="T40" s="66"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20">
       <c r="A41" s="30"/>
       <c r="B41" s="33"/>
       <c r="C41" s="114"/>
@@ -4045,7 +4040,7 @@
       <c r="S41" s="72"/>
       <c r="T41" s="66"/>
     </row>
-    <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="15.75" thickBot="1">
       <c r="A42" s="53"/>
       <c r="B42" s="54"/>
       <c r="C42" s="117"/>
@@ -4066,7 +4061,7 @@
       <c r="S42" s="69"/>
       <c r="T42" s="67"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20">
       <c r="H44" s="56"/>
       <c r="I44" s="56"/>
       <c r="J44" s="57" t="s">
@@ -4085,7 +4080,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20">
       <c r="H45" s="56"/>
       <c r="I45" s="56"/>
       <c r="J45" s="57" t="s">
@@ -4097,32 +4092,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20">
       <c r="G46" s="56"/>
       <c r="H46" s="56"/>
       <c r="I46" s="56"/>
       <c r="J46" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="L46" s="193" t="s">
+      <c r="L46" s="203" t="s">
         <v>31</v>
       </c>
-      <c r="M46" s="193"/>
-      <c r="N46" s="193"/>
-      <c r="O46" s="193"/>
-      <c r="P46" s="193"/>
-      <c r="Q46" s="193"/>
-      <c r="R46" s="193"/>
-      <c r="S46" s="193"/>
-      <c r="T46" s="193"/>
+      <c r="M46" s="203"/>
+      <c r="N46" s="203"/>
+      <c r="O46" s="203"/>
+      <c r="P46" s="203"/>
+      <c r="Q46" s="203"/>
+      <c r="R46" s="203"/>
+      <c r="S46" s="203"/>
+      <c r="T46" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="Q6:S7"/>
     <mergeCell ref="L46:T46"/>
@@ -4139,6 +4129,11 @@
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>